<commit_message>
Start Hypothesis Testing lesson in Udacity Inferential Stats
</commit_message>
<xml_diff>
--- a/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson2_Estimation.xlsx
+++ b/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson2_Estimation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="7416" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="7416"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>CI</t>
   </si>
@@ -149,7 +149,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +170,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -237,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -251,6 +258,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,15 +575,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +615,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>(40 - (2*16.04)/SQRT(35))</f>
         <v>34.57749030166184</v>
@@ -646,7 +656,7 @@
         <v>19.269253157511447</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>(40 + (2*16.04)/SQRT(35))</f>
         <v>45.42250969833816</v>
@@ -663,17 +673,17 @@
         <v>21.187889699631409</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I4">
         <v>15.4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I5">
         <v>21.4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>1</v>
       </c>
@@ -687,7 +697,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D7">
         <f>(16.04)/SQRT(250)</f>
         <v>1.014458673382016</v>
@@ -704,7 +714,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F8">
         <f>40+E7</f>
         <v>41.988338999828748</v>
@@ -713,7 +723,20 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="J11" s="7">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGE(J11:J17)</f>
+        <v>20.228571428571428</v>
+      </c>
+      <c r="L11">
+        <f>_xlfn.STDEV.P(J11:J17)</f>
+        <v>2.5381175733851657</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -726,8 +749,11 @@
       <c r="F12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J12" s="7">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>(40 - (2*16.04)/SQRT(35))</f>
         <v>34.57749030166184</v>
@@ -744,8 +770,29 @@
         <f>40-E13</f>
         <v>33.682776201436042</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J13" s="7">
+        <v>15.4</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="P13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="S13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>(40 + (2*16.04)/SQRT(35))</f>
         <v>45.42250969833816</v>
@@ -754,8 +801,57 @@
         <f>40+E13</f>
         <v>46.317223798563958</v>
       </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="J14" s="7">
+        <v>21.4</v>
+      </c>
+      <c r="L14">
+        <f>L11*1.96</f>
+        <v>4.9747104438349243</v>
+      </c>
+      <c r="M14">
+        <f>K11-L14</f>
+        <v>15.253860984736503</v>
+      </c>
+      <c r="O14">
+        <f>L11*2.33</f>
+        <v>5.9138139459874361</v>
+      </c>
+      <c r="P14">
+        <f>K11-O14</f>
+        <v>14.314757482583992</v>
+      </c>
+      <c r="R14">
+        <f>L11*2.575</f>
+        <v>6.5356527514668024</v>
+      </c>
+      <c r="S14">
+        <f>K11-R14</f>
+        <v>13.692918677104625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="J15" s="7">
+        <v>20.2</v>
+      </c>
+      <c r="M15">
+        <f>K11+L14</f>
+        <v>25.20328187240635</v>
+      </c>
+      <c r="P15">
+        <f>K11+O14</f>
+        <v>26.142385374558863</v>
+      </c>
+      <c r="S15">
+        <f>K11+R14</f>
+        <v>26.76422418003823</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="J16" s="7">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>1</v>
       </c>
@@ -765,8 +861,11 @@
       <c r="F17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="J17" s="7">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D18">
         <f>(16.04)/SQRT(250)</f>
         <v>1.014458673382016</v>
@@ -780,7 +879,7 @@
         <v>37.636311291019901</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
       <c r="F19">
         <f>40+E18</f>
         <v>42.363688708980099</v>
@@ -44516,8 +44615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>